<commit_message>
add Natinal Flags Hats
</commit_message>
<xml_diff>
--- a/CustomHatsGM.xlsx
+++ b/CustomHatsGM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -160,15 +160,6 @@
     <t xml:space="preserve">otono_climb.png</t>
   </si>
   <si>
-    <t xml:space="preserve">Matryoshka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matryoshka.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matryoshka_climb.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chu-ni</t>
   </si>
   <si>
@@ -197,6 +188,144 @@
   </si>
   <si>
     <t xml:space="preserve">kendama_flip_bounce_adaptive.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nationalFlagHat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">America.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">America_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">England</t>
+  </si>
+  <si>
+    <t xml:space="preserve">England.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">England_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistan.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistan_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seychelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seychelles.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seychelles_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri Lanka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SriLanka.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SriLanka_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine_climb.png</t>
   </si>
 </sst>
 </file>
@@ -322,7 +451,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -550,7 +679,7 @@
         <v>46</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>10</v>
@@ -567,7 +696,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>10</v>
@@ -584,7 +713,7 @@
         <v>52</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>10</v>
@@ -595,41 +724,265 @@
       <c r="F15" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="G15" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -693,7 +1046,7 @@
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Revert "Revert "update Hats""
This reverts commit 8974ad10e48e1401d54ed9a6990636679f554b61.
</commit_message>
<xml_diff>
--- a/CustomHatsGM.xlsx
+++ b/CustomHatsGM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="266">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -788,6 +788,36 @@
   </si>
   <si>
     <t xml:space="preserve">zennkopasu2_c.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myakumyaku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memeta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myakumyaku.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myakumyaku_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosamosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mosamosa_adaptive.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mosamosa_adaptive_climb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swan_adaptive.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swan_climb_adaptive.png</t>
   </si>
 </sst>
 </file>
@@ -912,8 +942,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2260,9 +2290,57 @@
         <v>255</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>